<commit_message>
Completed hydrogen sector draft structure (#296)
</commit_message>
<xml_diff>
--- a/InputData/hydgn/SYAHPC/Start Year Annual Hydrogen Production Capacity.xlsx
+++ b/InputData/hydgn/SYAHPC/Start Year Annual Hydrogen Production Capacity.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\SYAHPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF8D4EE-F5CC-4FEF-8735-78336A078F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FE882F-A74D-4DB1-BCD2-06FA36E25D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32250" yWindow="4155" windowWidth="24030" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60750" yWindow="1215" windowWidth="24900" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="SYAHPC" sheetId="3" r:id="rId2"/>
+    <sheet name="SYAHPC-green" sheetId="3" r:id="rId2"/>
+    <sheet name="SYAHPC-lowcarbon" sheetId="4" r:id="rId3"/>
+    <sheet name="SYAHPC-unspecified" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="btu_per_kwh">#REF!</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Source:</t>
   </si>
@@ -77,9 +79,6 @@
     <t>Start Year Annual Capacity</t>
   </si>
   <si>
-    <t>SYAHPC Start Year Annual Hydrogen Production Capacity</t>
-  </si>
-  <si>
     <t>indst/BIFU</t>
   </si>
   <si>
@@ -90,6 +89,15 @@
   </si>
   <si>
     <t xml:space="preserve"> (or higher if current production facilities are running under max capacity)</t>
+  </si>
+  <si>
+    <t>SYAHPC Start Year Annual Green Hydrogen Production Capacity</t>
+  </si>
+  <si>
+    <t>SYAHPC Start Year Annual Low Carbon Hydrogen Production Capacity</t>
+  </si>
+  <si>
+    <t>SYAHPC Start Year Annual Unspecified Hydrogen Production Capacity</t>
   </si>
 </sst>
 </file>
@@ -441,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,41 +462,51 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -526,6 +544,176 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F365724-3210-417D-AAD5-41339AA6285F}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86B67DC-846A-43A5-93A4-7633904409D9}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
         <v>39900000000000</v>
       </c>
     </row>

</xml_diff>